<commit_message>
worked on model to compute system matrices - but: EI is the same for all elastc structures. Must be updated in "WKA rev 10.mac"
</commit_message>
<xml_diff>
--- a/parameter.xlsx
+++ b/parameter.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hawhamburgedu-my.sharepoint.com/personal/wzo448_haw-hamburg_de/Documents/2025-SS/Maschinendynamik/Matlab/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hawhamburgedu-my.sharepoint.com/personal/wzo448_haw-hamburg_de/Documents/2025-SS/Maschinendynamik/Matlab/WKA0/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="114" documentId="13_ncr:1_{E0F3FCBD-CFA9-4B1E-9A8D-D887D26D3DC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CE511575-1405-4BF7-8804-059E74093FD9}"/>
+  <xr:revisionPtr revIDLastSave="305" documentId="13_ncr:1_{E0F3FCBD-CFA9-4B1E-9A8D-D887D26D3DC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1B36B7DC-DAC5-421B-A2EA-90CB7A60A8A2}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25180" windowHeight="16140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Systemparameter" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="62">
   <si>
     <t>=</t>
   </si>
@@ -56,12 +56,6 @@
     <t>geometry section</t>
   </si>
   <si>
-    <t>friction characteristic section (brake and asphalt)</t>
-  </si>
-  <si>
-    <t>initial values section</t>
-  </si>
-  <si>
     <t>solution parameters section</t>
   </si>
   <si>
@@ -71,9 +65,6 @@
     <t>m</t>
   </si>
   <si>
-    <t>Turmlänge</t>
-  </si>
-  <si>
     <t>l[B]</t>
   </si>
   <si>
@@ -89,24 +80,9 @@
     <t>m[B]</t>
   </si>
   <si>
-    <t>m[T]</t>
-  </si>
-  <si>
-    <t>Ip[T]</t>
-  </si>
-  <si>
     <t>D[T]</t>
   </si>
   <si>
-    <t>Außendurchmesser Turm</t>
-  </si>
-  <si>
-    <t>d[T]</t>
-  </si>
-  <si>
-    <t>Innendurchmesser Turm</t>
-  </si>
-  <si>
     <t>J[N,1]</t>
   </si>
   <si>
@@ -114,13 +90,145 @@
   </si>
   <si>
     <t>J[N,2]</t>
+  </si>
+  <si>
+    <t>tower</t>
+  </si>
+  <si>
+    <t>nacelle (rigid body)</t>
+  </si>
+  <si>
+    <t>rotor-shaft</t>
+  </si>
+  <si>
+    <t>center to bearing</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>bearing to rotor-center</t>
+  </si>
+  <si>
+    <t>rotor</t>
+  </si>
+  <si>
+    <t>m[R]</t>
+  </si>
+  <si>
+    <t>ρ[T]</t>
+  </si>
+  <si>
+    <t>kg/m^3</t>
+  </si>
+  <si>
+    <t>length tower</t>
+  </si>
+  <si>
+    <t>density tower</t>
+  </si>
+  <si>
+    <t>outer diameter</t>
+  </si>
+  <si>
+    <t>t[T]</t>
+  </si>
+  <si>
+    <t>cm</t>
+  </si>
+  <si>
+    <t>wall-thickness</t>
+  </si>
+  <si>
+    <t>kg*m^2</t>
+  </si>
+  <si>
+    <t>mass moment about 1-axis</t>
+  </si>
+  <si>
+    <t>mass moment about 2-axis</t>
+  </si>
+  <si>
+    <t>mass moment about 3-axis</t>
+  </si>
+  <si>
+    <t>nacelle-mass</t>
+  </si>
+  <si>
+    <t>kg</t>
+  </si>
+  <si>
+    <t>rotor-mass (without blades)</t>
+  </si>
+  <si>
+    <t>general</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>modulus of elasticity</t>
+  </si>
+  <si>
+    <t>N/m^2</t>
+  </si>
+  <si>
+    <t>D[S]</t>
+  </si>
+  <si>
+    <t>shaft-diameter</t>
+  </si>
+  <si>
+    <t>blade</t>
+  </si>
+  <si>
+    <t>N[0]</t>
+  </si>
+  <si>
+    <t>N[1]</t>
+  </si>
+  <si>
+    <t>ΔN</t>
+  </si>
+  <si>
+    <t>U/min</t>
+  </si>
+  <si>
+    <t>increment</t>
+  </si>
+  <si>
+    <t>start at ….</t>
+  </si>
+  <si>
+    <t>end at …</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         Ω = Oga for parameter variation</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>rotor-radius</t>
+  </si>
+  <si>
+    <t>EI[R]</t>
+  </si>
+  <si>
+    <t>N*m^2</t>
+  </si>
+  <si>
+    <t>blade-mass</t>
+  </si>
+  <si>
+    <t>bending stiffness blade</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -136,8 +244,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -147,6 +263,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39994506668294322"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -163,13 +285,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -185,6 +312,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -450,21 +581,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E43"/>
+  <dimension ref="A1:E34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.73046875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="1.796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.73046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="1.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -479,8 +610,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="4.5" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="3" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" ht="4.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -489,211 +620,423 @@
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A4" t="s">
+    <row r="4" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="2">
+        <v>210000000000</v>
+      </c>
+      <c r="D5" t="s">
+        <v>44</v>
+      </c>
+      <c r="E5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>120</v>
+      </c>
+      <c r="D8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>7800</v>
+      </c>
+      <c r="D9" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>10</v>
+      </c>
+      <c r="D10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>3</v>
+      </c>
+      <c r="D11" t="s">
+        <v>32</v>
+      </c>
+      <c r="E11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>5000</v>
+      </c>
+      <c r="D13" t="s">
+        <v>39</v>
+      </c>
+      <c r="E13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" t="s">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <f>C13*3^2</f>
+        <v>45000</v>
+      </c>
+      <c r="D14" t="s">
+        <v>34</v>
+      </c>
+      <c r="E14" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <f>C13*3^2</f>
+        <v>45000</v>
+      </c>
+      <c r="D15" t="s">
+        <v>34</v>
+      </c>
+      <c r="E15" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" t="s">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <f>C13*3^2</f>
+        <v>45000</v>
+      </c>
+      <c r="D16" t="s">
+        <v>34</v>
+      </c>
+      <c r="E16" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>4</v>
+      </c>
+      <c r="D17" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" t="s">
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <v>3</v>
+      </c>
+      <c r="D19" t="s">
+        <v>8</v>
+      </c>
+      <c r="E19" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>45</v>
+      </c>
+      <c r="B20" t="s">
+        <v>0</v>
+      </c>
+      <c r="C20">
+        <v>2</v>
+      </c>
+      <c r="D20" t="s">
+        <v>8</v>
+      </c>
+      <c r="E20" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>25</v>
+      </c>
+      <c r="B23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C23">
+        <v>1000</v>
+      </c>
+      <c r="D23" t="s">
+        <v>39</v>
+      </c>
+      <c r="E23" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>56</v>
+      </c>
+      <c r="B24" t="s">
+        <v>0</v>
+      </c>
+      <c r="C24">
+        <v>4</v>
+      </c>
+      <c r="D24" t="s">
+        <v>8</v>
+      </c>
+      <c r="E24" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>58</v>
+      </c>
+      <c r="B25" t="s">
+        <v>0</v>
+      </c>
+      <c r="C25" s="2">
+        <v>1000000</v>
+      </c>
+      <c r="D25" t="s">
+        <v>59</v>
+      </c>
+      <c r="E25" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
         <v>9</v>
       </c>
-      <c r="B4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4">
-        <v>120</v>
-      </c>
-      <c r="D4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="B27" t="s">
+        <v>0</v>
+      </c>
+      <c r="C27">
+        <v>70</v>
+      </c>
+      <c r="D27" t="s">
+        <v>8</v>
+      </c>
+      <c r="E27" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5">
-        <v>70</v>
-      </c>
-      <c r="D5" t="s">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
         <v>13</v>
       </c>
-      <c r="E5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A8" t="s">
-        <v>19</v>
-      </c>
-      <c r="E8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A9" t="s">
-        <v>21</v>
-      </c>
-      <c r="E9" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="C10" s="2"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="C11" s="2"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="C12" s="2"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="C13" s="2"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="C14" s="2"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="C15" s="2"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="C16" s="2"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A17" t="s">
-        <v>17</v>
-      </c>
-      <c r="C17" s="2"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A18" t="s">
-        <v>18</v>
-      </c>
-      <c r="B18" t="s">
-        <v>0</v>
-      </c>
-      <c r="C18" s="2"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A19" t="s">
-        <v>15</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C19" s="2"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A20" t="s">
-        <v>23</v>
-      </c>
-      <c r="C20" s="2"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A21" t="s">
-        <v>25</v>
-      </c>
-      <c r="C21" s="2"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A22" t="s">
-        <v>24</v>
-      </c>
-      <c r="C22" s="2"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A23" t="s">
-        <v>16</v>
-      </c>
-      <c r="C23" s="2"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="C24" s="2"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A25" s="1" t="s">
+      <c r="B28" t="s">
+        <v>0</v>
+      </c>
+      <c r="C28" s="2">
+        <v>10000</v>
+      </c>
+      <c r="D28" t="s">
+        <v>39</v>
+      </c>
+      <c r="E28" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A29" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>48</v>
+      </c>
+      <c r="B30" t="s">
+        <v>0</v>
+      </c>
+      <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="D30" t="s">
+        <v>51</v>
+      </c>
+      <c r="E30" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>49</v>
+      </c>
+      <c r="B31" t="s">
+        <v>0</v>
+      </c>
+      <c r="C31">
+        <v>1</v>
+      </c>
+      <c r="D31" t="s">
+        <v>51</v>
+      </c>
+      <c r="E31" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>50</v>
+      </c>
+      <c r="B32" t="s">
+        <v>0</v>
+      </c>
+      <c r="C32">
+        <v>0.1</v>
+      </c>
+      <c r="D32" t="s">
+        <v>51</v>
+      </c>
+      <c r="E32" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A33" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="C26" s="2"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="C27" s="2"/>
-      <c r="D27" s="3"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="C28" s="2"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="C29" s="2"/>
-      <c r="D29" s="3"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="C30" s="2"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="C31" s="2"/>
-      <c r="D31" s="3"/>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="C32" s="2"/>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="C33" s="2"/>
-      <c r="D33" s="3"/>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C34" s="2"/>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="C35" s="2"/>
-      <c r="D35" s="3"/>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="C36" s="2"/>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="C37" s="2"/>
-      <c r="D37" s="3"/>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="C38" s="2"/>
-      <c r="D38" s="3"/>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="C39" s="2"/>
-      <c r="D39" s="3"/>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A40" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B40" s="1"/>
-      <c r="C40" s="1"/>
-      <c r="D40" s="1"/>
-      <c r="E40" s="1"/>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="C41" s="2"/>
-      <c r="D41" s="3"/>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A42" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B42" s="1"/>
-      <c r="C42" s="1"/>
-      <c r="D42" s="1"/>
-      <c r="E42" s="1"/>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="C43" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
corrected minor mistakes - still the system "explodes"
</commit_message>
<xml_diff>
--- a/parameter.xlsx
+++ b/parameter.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hawhamburgedu-my.sharepoint.com/personal/wzo448_haw-hamburg_de/Documents/2025-SS/Maschinendynamik/Matlab/WKA0/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="384" documentId="13_ncr:1_{E0F3FCBD-CFA9-4B1E-9A8D-D887D26D3DC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{84C3775B-C8A2-44D2-8CDC-3BD5E2DFCB7D}"/>
+  <xr:revisionPtr revIDLastSave="392" documentId="13_ncr:1_{E0F3FCBD-CFA9-4B1E-9A8D-D887D26D3DC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F8DDCF56-9C6B-41D5-AEEA-1BDA3F06FE09}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25180" windowHeight="16140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -351,6 +351,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -618,8 +622,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -889,7 +893,7 @@
         <v>0</v>
       </c>
       <c r="C21">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D21" t="s">
         <v>8</v>
@@ -906,7 +910,7 @@
         <v>0</v>
       </c>
       <c r="C22">
-        <v>1</v>
+        <v>0.3</v>
       </c>
       <c r="D22" t="s">
         <v>8</v>
@@ -1061,7 +1065,7 @@
         <v>0</v>
       </c>
       <c r="C32" s="2">
-        <v>0.1</v>
+        <v>3</v>
       </c>
       <c r="D32" t="s">
         <v>62</v>
@@ -1079,7 +1083,7 @@
       </c>
       <c r="C33" s="2">
         <f>C30*C29^3*(2*PI()*C32)^2/20</f>
-        <v>67705486.191472992</v>
+        <v>60934937572.325699</v>
       </c>
       <c r="D33" t="s">
         <v>57</v>
@@ -1099,7 +1103,7 @@
         <v>0</v>
       </c>
       <c r="C34" s="2">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="D34" t="s">
         <v>66</v>
@@ -1125,7 +1129,7 @@
         <v>0</v>
       </c>
       <c r="C36">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="D36" t="s">
         <v>50</v>

</xml_diff>

<commit_message>
delivers plausible results - first time ....
</commit_message>
<xml_diff>
--- a/parameter.xlsx
+++ b/parameter.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hawhamburgedu-my.sharepoint.com/personal/wzo448_haw-hamburg_de/Documents/2025-SS/Maschinendynamik/Matlab/WKA0/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="392" documentId="13_ncr:1_{E0F3FCBD-CFA9-4B1E-9A8D-D887D26D3DC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F8DDCF56-9C6B-41D5-AEEA-1BDA3F06FE09}"/>
+  <xr:revisionPtr revIDLastSave="398" documentId="13_ncr:1_{E0F3FCBD-CFA9-4B1E-9A8D-D887D26D3DC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9A6DD241-3930-47AA-A7C8-BE2CEA9B139A}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25180" windowHeight="16140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -351,10 +351,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -623,7 +619,7 @@
   <dimension ref="A1:G40"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -770,7 +766,7 @@
         <v>0</v>
       </c>
       <c r="C13">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D13" t="s">
         <v>32</v>
@@ -1129,7 +1125,7 @@
         <v>0</v>
       </c>
       <c r="C36">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="D36" t="s">
         <v>50</v>
@@ -1146,7 +1142,7 @@
         <v>0</v>
       </c>
       <c r="C37">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="D37" t="s">
         <v>50</v>
@@ -1163,7 +1159,7 @@
         <v>0</v>
       </c>
       <c r="C38">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D38" t="s">
         <v>50</v>

</xml_diff>

<commit_message>
voll einsatzfähige Version; die charakteristischen Multiplikatoren stehen in C.mat
</commit_message>
<xml_diff>
--- a/parameter.xlsx
+++ b/parameter.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hawhamburgedu-my.sharepoint.com/personal/wzo448_haw-hamburg_de/Documents/2025-SS/Maschinendynamik/Matlab/WKA0/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="398" documentId="13_ncr:1_{E0F3FCBD-CFA9-4B1E-9A8D-D887D26D3DC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9A6DD241-3930-47AA-A7C8-BE2CEA9B139A}"/>
+  <xr:revisionPtr revIDLastSave="404" documentId="13_ncr:1_{E0F3FCBD-CFA9-4B1E-9A8D-D887D26D3DC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D972A53A-569B-4233-8D55-F4A14D2893D4}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25180" windowHeight="16140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="76">
   <si>
     <t>=</t>
   </si>
@@ -261,6 +261,9 @@
   </si>
   <si>
     <t>shear modulus</t>
+  </si>
+  <si>
+    <t>= 12 sek / U</t>
   </si>
 </sst>
 </file>
@@ -324,7 +327,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -336,6 +339,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -351,6 +355,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -619,7 +627,7 @@
   <dimension ref="A1:G40"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1125,7 +1133,7 @@
         <v>0</v>
       </c>
       <c r="C36">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D36" t="s">
         <v>50</v>
@@ -1142,13 +1150,16 @@
         <v>0</v>
       </c>
       <c r="C37">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D37" t="s">
         <v>50</v>
       </c>
       <c r="E37" t="s">
         <v>53</v>
+      </c>
+      <c r="G37" s="5" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.35">
@@ -1159,7 +1170,7 @@
         <v>0</v>
       </c>
       <c r="C38">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D38" t="s">
         <v>50</v>

</xml_diff>